<commit_message>
update new script for couinaud segment segmentation
</commit_message>
<xml_diff>
--- a/eval_mean_whole_liver_PDFF.xlsx
+++ b/eval_mean_whole_liver_PDFF.xlsx
@@ -1281,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9029A9EA-E686-41D1-B42C-01C4A5E80E0D}">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:S45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>